<commit_message>
updaeted the site layout
e
</commit_message>
<xml_diff>
--- a/things that aren't the website/site layout.xlsx
+++ b/things that aren't the website/site layout.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattw\Documents\Year 9 IST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\OneDrive\Desktop\Work\ICT\Bullying Assignment\things that aren't the website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B3E1260-7984-49EA-A020-26836C972B52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{9B3E1260-7984-49EA-A020-26836C972B52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{C667E647-DB31-41FA-9DC8-972B07715218}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EC3C515D-4DA3-4661-BE28-CBB9921FF436}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{EC3C515D-4DA3-4661-BE28-CBB9921FF436}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="home page and main titles" sheetId="1" r:id="rId1"/>
+    <sheet name="What is bullying" sheetId="2" r:id="rId2"/>
+    <sheet name="What can I do" sheetId="3" r:id="rId3"/>
+    <sheet name="subbages e.g (Cyperbullying)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="16">
   <si>
     <t>LOGO</t>
   </si>
@@ -54,6 +55,33 @@
   </si>
   <si>
     <t>Image</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Verbal</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>Cyber</t>
+  </si>
+  <si>
+    <t>If I'm Getting Bullied</t>
+  </si>
+  <si>
+    <t>If I See Someone Getting Bullied</t>
+  </si>
+  <si>
+    <t>Images</t>
   </si>
 </sst>
 </file>
@@ -76,7 +104,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +132,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -237,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -261,6 +295,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,13 +628,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99247FFE-7CB8-459D-8E9B-2A8A336CE241}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +646,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -605,7 +656,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -617,7 +668,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
@@ -633,7 +684,7 @@
       <c r="G4" s="22"/>
       <c r="H4" s="21"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
       <c r="B5" s="13"/>
       <c r="C5" s="12" t="s">
@@ -655,7 +706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="16"/>
       <c r="C6" s="15" t="s">
@@ -677,7 +728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
@@ -701,7 +752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="14"/>
       <c r="B8" s="16"/>
       <c r="C8" s="15" t="s">
@@ -723,7 +774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="19"/>
       <c r="C9" s="15" t="s">
@@ -745,7 +796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>5</v>
       </c>
@@ -771,7 +822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>5</v>
       </c>
@@ -797,7 +848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>5</v>
       </c>
@@ -823,7 +874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>5</v>
       </c>
@@ -849,7 +900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>5</v>
       </c>
@@ -875,7 +926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>5</v>
       </c>
@@ -897,7 +948,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>5</v>
       </c>
@@ -921,7 +972,7 @@
       </c>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>5</v>
       </c>
@@ -943,7 +994,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
         <v>5</v>
       </c>
@@ -965,7 +1016,7 @@
       <c r="G18" s="17"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
         <v>2</v>
       </c>
@@ -985,4 +1036,1311 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A65C29-2C9A-4428-B549-16EDC78FD4A4}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="38"/>
+      <c r="E5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="38"/>
+      <c r="G5" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="38"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2F1849-36A3-424F-9A34-81395120F351}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="38"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C79E6DE-8E7F-4CFD-9763-48AD0080ACC9}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="38"/>
+      <c r="E5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="38"/>
+      <c r="G5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>